<commit_message>
file for 9 comparisons
</commit_message>
<xml_diff>
--- a/01_Paradigms/ER-ED/ER_ED/VS1_Rounds.xlsx
+++ b/01_Paradigms/ER-ED/ER_ED/VS1_Rounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\04_Projekte\01_COG-ED_Revision\CAD\01_Paradigms\COG-ED\Stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_CERED\CAD\01_Paradigms\ER-ED\ER_ED\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -344,11 +344,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -402,51 +400,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>